<commit_message>
updated the file to reflex current headers for the various trait data file
</commit_message>
<xml_diff>
--- a/benthic/data_output/traits/trait_column_comp.xlsx
+++ b/benthic/data_output/traits/trait_column_comp.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositories\drought_traits\benthic\data_output\traits\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61F46550-C49F-48FA-9CA4-5F0AA874182A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6A5D6FC-E964-48E7-A1CF-E51C06D79E51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{93C2C434-7D14-4090-8A3E-1B1238F9BC0C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{93C2C434-7D14-4090-8A3E-1B1238F9BC0C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="32">
   <si>
     <t>organism_code</t>
   </si>
@@ -107,27 +107,9 @@
     <t>aphia_id</t>
   </si>
   <si>
-    <t>taxon</t>
-  </si>
-  <si>
-    <t>rank</t>
-  </si>
-  <si>
-    <t>units</t>
-  </si>
-  <si>
     <t>life_stage</t>
   </si>
   <si>
-    <t>body_dimension</t>
-  </si>
-  <si>
-    <t>body_measure_type</t>
-  </si>
-  <si>
-    <t>trait_database</t>
-  </si>
-  <si>
     <t>quality_status</t>
   </si>
   <si>
@@ -149,10 +131,7 @@
     <t>matching</t>
   </si>
   <si>
-    <t>usgs and nemesis are good enough match for now</t>
-  </si>
-  <si>
-    <t>just need to work on formatting of worms a bit (reorder and rename columns)</t>
+    <t>iep</t>
   </si>
 </sst>
 </file>
@@ -168,7 +147,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -193,6 +172,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -206,12 +191,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -526,46 +512,45 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CA50859-0795-4576-BCBB-FD43C68E8322}">
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.08984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.5703125" customWidth="1"/>
+    <col min="6" max="6" width="22.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>21</v>
       </c>
       <c r="B1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="C2" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C2" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="G2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
@@ -575,184 +560,241 @@
       <c r="C3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
       <c r="B10" s="4"/>
-      <c r="C10" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D10" s="4"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
       <c r="B11" s="4"/>
-      <c r="C11" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D11" s="4"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
       <c r="B12" s="4"/>
-      <c r="C12" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D12" s="4"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>10</v>
       </c>
       <c r="B13" s="4"/>
-      <c r="C13" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D13" s="4"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C14" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B15" s="4"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C15"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C16" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C17"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C18"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C19"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A21" s="3" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C21" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B22" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A22" s="3" t="s">
+      <c r="C22" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B23" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A23" s="3" t="s">
+      <c r="C23" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B24" s="3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B24" s="1" t="s">
-        <v>33</v>
+      <c r="C24" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B25" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C26" s="5" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>